<commit_message>
Feito traduções no vixi-website
</commit_message>
<xml_diff>
--- a/database/translations.xlsx
+++ b/database/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\leebank\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43085690-ABE8-42A5-B948-2F15429DD873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DCCE91-EEA3-4134-B82F-310AEF7EA96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-210" windowWidth="20640" windowHeight="11160" xr2:uid="{76BFD47B-F395-40CE-A23A-1FAE0D23D331}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="124">
   <si>
     <t>id</t>
   </si>
@@ -268,6 +268,144 @@
   </si>
   <si>
     <t>Voltar à Homepage</t>
+  </si>
+  <si>
+    <t>Guiding you</t>
+  </si>
+  <si>
+    <t>for your future</t>
+  </si>
+  <si>
+    <t>We have come to inspire people to go further, to achieve their dreams, through a partnership of trust that grows every day.</t>
+  </si>
+  <si>
+    <t>We are synonymous with competence, reliability, and accessibility.</t>
+  </si>
+  <si>
+    <t>We want our customers to have the exact feeling that they can count on us and that our product meets their expectations and needs.</t>
+  </si>
+  <si>
+    <t>VIXI's OTC desk has a liquidity offering that guarantees institutional customers the desired amount of Bitcoin, Ethereum, Decred, Stablecoins and other digital assets.</t>
+  </si>
+  <si>
+    <t>Main problems solved by VIXI's OTC desk:</t>
+  </si>
+  <si>
+    <t>The time difference between the time of the order and its settlement often incurs a difference in the initial price due to the size of the order.</t>
+  </si>
+  <si>
+    <t>Trading Limits</t>
+  </si>
+  <si>
+    <t>It is common for large exchanges to impose daily trading and trading limits to maintain their liquidity. For high-volume clients this practice is inappropriate.</t>
+  </si>
+  <si>
+    <t>Learn More</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>We value a relationship of trust and transparency with our customers. Because of this, the data security and privacy of our users is of utmost importance to us.</t>
+  </si>
+  <si>
+    <t>Our Compliance policy follows all LGPD standards, and offers absolute confidentiality about you and your coins. We also have a highly trained digital security team.</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Fill in the fields below to</t>
+  </si>
+  <si>
+    <t>the registration request</t>
+  </si>
+  <si>
+    <t>Request Registration</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>OTC, or over-the-counter, refers to the time when assets were traded over the counter at brokerage houses. The process offers less bureaucracy and allows more direct negotiations between buyers and sellers, enabling the investor to find more opportunities when buying currencies.</t>
+  </si>
+  <si>
+    <t>For large quantity trading, OTC trading mainly provides the following advantages</t>
+  </si>
+  <si>
+    <t>Saving Money</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>Great limits</t>
+  </si>
+  <si>
+    <t>One of the most important, in OTC transactions there is an agreement on a price that is beneficial to both parties and that does not need to correspond to the market price. This creates a WIN-WIN scenario for those involved.</t>
+  </si>
+  <si>
+    <t>The market will not see variations, concealing their intentions to enter or exit. Moreover, with a trusted intermediary between the counterparties, they do not need to reveal their identities, being the only one who knows both sides.</t>
+  </si>
+  <si>
+    <t>It is not tied to participation on an exchange under fixed rules. This guarantees traders the ability to trade securities more broadly and without the low limits of traditional platforms.</t>
+  </si>
+  <si>
+    <t>Back to Homepage</t>
+  </si>
+  <si>
+    <t>vixiTel</t>
+  </si>
+  <si>
+    <t>Tel</t>
+  </si>
+  <si>
+    <t>vixiAddress</t>
+  </si>
+  <si>
+    <t>Endereço da Empresa</t>
+  </si>
+  <si>
+    <t>Company Address</t>
+  </si>
+  <si>
+    <t>vixiPrivacyPolice</t>
+  </si>
+  <si>
+    <t>Política de Privacidade</t>
+  </si>
+  <si>
+    <t>Privacy Policy</t>
+  </si>
+  <si>
+    <t>vixiTerms</t>
+  </si>
+  <si>
+    <t>Termos de uso</t>
+  </si>
+  <si>
+    <t>Terms of Use</t>
+  </si>
+  <si>
+    <t>vixiHelp</t>
+  </si>
+  <si>
+    <t>Central de Ajuda</t>
+  </si>
+  <si>
+    <t>Help Center</t>
+  </si>
+  <si>
+    <t>vixiAllRights</t>
+  </si>
+  <si>
+    <t>© Razão Social da VIXI, 2022. Todos os direitos reservados</t>
+  </si>
+  <si>
+    <t>© VIXI Corporate Name, 2022. All rights reserved</t>
   </si>
 </sst>
 </file>
@@ -303,9 +441,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02064365-2FF8-4B03-A006-514EE9525724}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,6 +795,9 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
@@ -669,6 +809,9 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
@@ -680,6 +823,9 @@
       <c r="B4" t="s">
         <v>10</v>
       </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
@@ -691,6 +837,9 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
@@ -702,6 +851,9 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
@@ -713,6 +865,9 @@
       <c r="B7" t="s">
         <v>17</v>
       </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
@@ -724,6 +879,9 @@
       <c r="B8" t="s">
         <v>37</v>
       </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
@@ -735,6 +893,9 @@
       <c r="B9" t="s">
         <v>19</v>
       </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
@@ -746,6 +907,9 @@
       <c r="B10" t="s">
         <v>21</v>
       </c>
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
@@ -757,6 +921,9 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
       <c r="D11" t="s">
         <v>4</v>
       </c>
@@ -768,6 +935,9 @@
       <c r="B12" t="s">
         <v>25</v>
       </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
       <c r="D12" t="s">
         <v>4</v>
       </c>
@@ -779,6 +949,9 @@
       <c r="B13" t="s">
         <v>27</v>
       </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
       <c r="D13" t="s">
         <v>4</v>
       </c>
@@ -790,6 +963,9 @@
       <c r="B14" t="s">
         <v>29</v>
       </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
       <c r="D14" t="s">
         <v>4</v>
       </c>
@@ -801,6 +977,9 @@
       <c r="B15" t="s">
         <v>31</v>
       </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
       <c r="D15" t="s">
         <v>4</v>
       </c>
@@ -812,6 +991,9 @@
       <c r="B16" t="s">
         <v>34</v>
       </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
       <c r="D16" t="s">
         <v>4</v>
       </c>
@@ -823,6 +1005,9 @@
       <c r="B17" t="s">
         <v>35</v>
       </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
       <c r="D17" t="s">
         <v>4</v>
       </c>
@@ -834,6 +1019,9 @@
       <c r="B18" t="s">
         <v>39</v>
       </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
       <c r="D18" t="s">
         <v>4</v>
       </c>
@@ -845,6 +1033,9 @@
       <c r="B19" t="s">
         <v>41</v>
       </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
       <c r="D19" t="s">
         <v>4</v>
       </c>
@@ -856,6 +1047,9 @@
       <c r="B20" t="s">
         <v>43</v>
       </c>
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
       <c r="D20" t="s">
         <v>4</v>
       </c>
@@ -867,6 +1061,9 @@
       <c r="B21" t="s">
         <v>45</v>
       </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
       <c r="D21" t="s">
         <v>4</v>
       </c>
@@ -878,6 +1075,9 @@
       <c r="B22" t="s">
         <v>47</v>
       </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
       <c r="D22" t="s">
         <v>4</v>
       </c>
@@ -889,6 +1089,9 @@
       <c r="B23" t="s">
         <v>49</v>
       </c>
+      <c r="C23" t="s">
+        <v>95</v>
+      </c>
       <c r="D23" t="s">
         <v>4</v>
       </c>
@@ -900,6 +1103,9 @@
       <c r="B24" t="s">
         <v>55</v>
       </c>
+      <c r="C24" t="s">
+        <v>96</v>
+      </c>
       <c r="D24" t="s">
         <v>4</v>
       </c>
@@ -911,6 +1117,9 @@
       <c r="B25" t="s">
         <v>56</v>
       </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
       <c r="D25" t="s">
         <v>4</v>
       </c>
@@ -922,6 +1131,9 @@
       <c r="B26" t="s">
         <v>57</v>
       </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
       <c r="D26" t="s">
         <v>4</v>
       </c>
@@ -933,6 +1145,9 @@
       <c r="B27" t="s">
         <v>58</v>
       </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
       <c r="D27" t="s">
         <v>4</v>
       </c>
@@ -944,6 +1159,9 @@
       <c r="B28" t="s">
         <v>59</v>
       </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
       <c r="D28" t="s">
         <v>4</v>
       </c>
@@ -955,6 +1173,9 @@
       <c r="B29" t="s">
         <v>61</v>
       </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
@@ -966,6 +1187,9 @@
       <c r="B30" t="s">
         <v>63</v>
       </c>
+      <c r="C30" t="s">
+        <v>99</v>
+      </c>
       <c r="D30" t="s">
         <v>4</v>
       </c>
@@ -977,6 +1201,9 @@
       <c r="B31" t="s">
         <v>67</v>
       </c>
+      <c r="C31" t="s">
+        <v>100</v>
+      </c>
       <c r="D31" t="s">
         <v>4</v>
       </c>
@@ -988,67 +1215,166 @@
       <c r="B32" t="s">
         <v>68</v>
       </c>
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
       <c r="D32" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
       <c r="B33" t="s">
         <v>69</v>
       </c>
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
       <c r="D33" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>70</v>
       </c>
       <c r="B34" t="s">
         <v>71</v>
       </c>
+      <c r="C34" t="s">
+        <v>103</v>
+      </c>
       <c r="D34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
       <c r="B35" t="s">
         <v>73</v>
       </c>
+      <c r="C35" t="s">
+        <v>104</v>
+      </c>
       <c r="D35" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>74</v>
       </c>
       <c r="B36" t="s">
         <v>75</v>
       </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
       <c r="D36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>76</v>
       </c>
       <c r="B37" t="s">
         <v>77</v>
       </c>
+      <c r="C37" t="s">
+        <v>106</v>
+      </c>
       <c r="D37" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F38" s="1"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Efetuado correções leebank de acordo com o pdf "Apresentação problemas do site lee bank"
</commit_message>
<xml_diff>
--- a/database/translations.xlsx
+++ b/database/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\leebank\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\leebank\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A187395-9EC0-45AC-9C78-37A692F5D260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65822CEA-A30B-4D14-8997-904701D7B388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-210" windowWidth="20640" windowHeight="11160" xr2:uid="{76BFD47B-F395-40CE-A23A-1FAE0D23D331}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{76BFD47B-F395-40CE-A23A-1FAE0D23D331}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="161">
   <si>
     <t>id</t>
   </si>
@@ -508,6 +508,15 @@
   </si>
   <si>
     <t>返回首页</t>
+  </si>
+  <si>
+    <t>findInAClick</t>
+  </si>
+  <si>
+    <t>encontre num clique</t>
+  </si>
+  <si>
+    <t>find in a click</t>
   </si>
 </sst>
 </file>
@@ -859,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02064365-2FF8-4B03-A006-514EE9525724}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,6 +1484,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" t="s">
+        <v>159</v>
+      </c>
+      <c r="C44" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tradução em em chines acrescentada
</commit_message>
<xml_diff>
--- a/database/translations.xlsx
+++ b/database/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\leebank\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\leebank\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147A77E7-980E-410E-B724-FBE81E83BDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263952A5-4452-401A-81BA-116439C4EF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{76BFD47B-F395-40CE-A23A-1FAE0D23D331}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="168">
   <si>
     <t>id</t>
   </si>
@@ -523,14 +523,37 @@
   </si>
   <si>
     <t>Voltar para Homepage</t>
+  </si>
+  <si>
+    <t>公司地址</t>
+  </si>
+  <si>
+    <t>隐私权政策</t>
+  </si>
+  <si>
+    <t>使用条款</t>
+  </si>
+  <si>
+    <t>帮助中心</t>
+  </si>
+  <si>
+    <t>© VIXI 公司名称，2022。版权所有</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -558,8 +581,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,7 +901,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,8 +1440,8 @@
       <c r="C38" t="s">
         <v>96</v>
       </c>
-      <c r="D38" t="s">
-        <v>4</v>
+      <c r="D38" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,8 +1454,8 @@
       <c r="C39" t="s">
         <v>110</v>
       </c>
-      <c r="D39" t="s">
-        <v>4</v>
+      <c r="D39" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1444,8 +1468,8 @@
       <c r="C40" t="s">
         <v>113</v>
       </c>
-      <c r="D40" t="s">
-        <v>4</v>
+      <c r="D40" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,8 +1482,8 @@
       <c r="C41" t="s">
         <v>116</v>
       </c>
-      <c r="D41" t="s">
-        <v>4</v>
+      <c r="D41" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1472,8 +1496,8 @@
       <c r="C42" t="s">
         <v>119</v>
       </c>
-      <c r="D42" t="s">
-        <v>4</v>
+      <c r="D42" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,8 +1510,8 @@
       <c r="C43" t="s">
         <v>122</v>
       </c>
-      <c r="D43" t="s">
-        <v>4</v>
+      <c r="D43" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tradução dos titulos e alteração de horas
</commit_message>
<xml_diff>
--- a/database/translations.xlsx
+++ b/database/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\leebank\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\leebank\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A25DF2-71E4-4807-B76B-17226BCB819F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B797210B-4B46-43AB-9445-3E59D309DBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{76BFD47B-F395-40CE-A23A-1FAE0D23D331}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{76BFD47B-F395-40CE-A23A-1FAE0D23D331}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3314" uniqueCount="2359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3330" uniqueCount="2367">
   <si>
     <t>id</t>
   </si>
@@ -6426,9 +6426,6 @@
     <t>PROCEDIMENTO KNOW YOUR PARTNER – KYP</t>
   </si>
   <si>
-    <t>PROCEDIMENTO CONHEÇA O SEU PARCEIRO - KYP</t>
-  </si>
-  <si>
     <t>vixiCsKypDate</t>
   </si>
   <si>
@@ -7111,6 +7108,33 @@
   </si>
   <si>
     <t>vixiCsKypClassComp</t>
+  </si>
+  <si>
+    <t>vixiCsCompliance</t>
+  </si>
+  <si>
+    <t>vixiCsProcedimentos</t>
+  </si>
+  <si>
+    <t>Políticas adotadas pela empresa.</t>
+  </si>
+  <si>
+    <t>Policies adopted by the company.</t>
+  </si>
+  <si>
+    <t>vixiCsSeguranca</t>
+  </si>
+  <si>
+    <t>vixiCsPoliticas</t>
+  </si>
+  <si>
+    <t>Procedimentos</t>
+  </si>
+  <si>
+    <t>Procedures</t>
+  </si>
+  <si>
+    <t>PROCEDURE KNOW YOUR PARTNER - KYP</t>
   </si>
 </sst>
 </file>
@@ -7472,10 +7496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02064365-2FF8-4B03-A006-514EE9525724}">
-  <dimension ref="A1:D839"/>
+  <dimension ref="A1:E844"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A461" workbookViewId="0">
-      <selection activeCell="E626" sqref="E626"/>
+    <sheetView tabSelected="1" topLeftCell="A742" workbookViewId="0">
+      <selection activeCell="A750" sqref="A750"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17882,7 +17906,7 @@
         <v>2129</v>
       </c>
       <c r="C750" t="s">
-        <v>2130</v>
+        <v>2366</v>
       </c>
       <c r="D750" t="s">
         <v>4</v>
@@ -17890,7 +17914,7 @@
     </row>
     <row r="751" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="B751" s="2">
         <v>44350</v>
@@ -17904,7 +17928,7 @@
     </row>
     <row r="752" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="B752" t="s">
         <v>173</v>
@@ -17918,13 +17942,13 @@
     </row>
     <row r="753" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A753" t="s">
+        <v>2132</v>
+      </c>
+      <c r="B753" t="s">
         <v>2133</v>
       </c>
-      <c r="B753" t="s">
+      <c r="C753" t="s">
         <v>2134</v>
-      </c>
-      <c r="C753" t="s">
-        <v>2135</v>
       </c>
       <c r="D753" t="s">
         <v>4</v>
@@ -17932,7 +17956,7 @@
     </row>
     <row r="754" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="B754" t="s">
         <v>182</v>
@@ -17946,13 +17970,13 @@
     </row>
     <row r="755" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
+        <v>2136</v>
+      </c>
+      <c r="B755" t="s">
         <v>2137</v>
       </c>
-      <c r="B755" t="s">
+      <c r="C755" t="s">
         <v>2138</v>
-      </c>
-      <c r="C755" t="s">
-        <v>2139</v>
       </c>
       <c r="D755" t="s">
         <v>4</v>
@@ -17960,7 +17984,7 @@
     </row>
     <row r="756" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="B756" t="s">
         <v>188</v>
@@ -17974,7 +17998,7 @@
     </row>
     <row r="757" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="B757" t="s">
         <v>191</v>
@@ -17988,13 +18012,13 @@
     </row>
     <row r="758" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
+        <v>2141</v>
+      </c>
+      <c r="B758" t="s">
         <v>2142</v>
       </c>
-      <c r="B758" t="s">
-        <v>2143</v>
-      </c>
       <c r="C758" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="D758" t="s">
         <v>4</v>
@@ -18002,7 +18026,7 @@
     </row>
     <row r="759" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="B759" t="s">
         <v>1786</v>
@@ -18016,13 +18040,13 @@
     </row>
     <row r="760" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
+        <v>2144</v>
+      </c>
+      <c r="B760" t="s">
         <v>2145</v>
       </c>
-      <c r="B760" t="s">
+      <c r="C760" t="s">
         <v>2146</v>
-      </c>
-      <c r="C760" t="s">
-        <v>2147</v>
       </c>
       <c r="D760" t="s">
         <v>4</v>
@@ -18030,7 +18054,7 @@
     </row>
     <row r="761" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="B761" t="s">
         <v>1790</v>
@@ -18044,7 +18068,7 @@
     </row>
     <row r="762" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A762" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="B762" t="s">
         <v>1619</v>
@@ -18058,13 +18082,13 @@
     </row>
     <row r="763" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
+        <v>2149</v>
+      </c>
+      <c r="B763" t="s">
         <v>2150</v>
       </c>
-      <c r="B763" t="s">
+      <c r="C763" t="s">
         <v>2151</v>
-      </c>
-      <c r="C763" t="s">
-        <v>2152</v>
       </c>
       <c r="D763" t="s">
         <v>4</v>
@@ -18072,7 +18096,7 @@
     </row>
     <row r="764" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="B764" t="s">
         <v>1624</v>
@@ -18086,13 +18110,13 @@
     </row>
     <row r="765" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
+        <v>2153</v>
+      </c>
+      <c r="B765" t="s">
         <v>2154</v>
       </c>
-      <c r="B765" t="s">
+      <c r="C765" t="s">
         <v>2155</v>
-      </c>
-      <c r="C765" t="s">
-        <v>2156</v>
       </c>
       <c r="D765" t="s">
         <v>4</v>
@@ -18100,7 +18124,7 @@
     </row>
     <row r="766" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="B766" t="s">
         <v>1630</v>
@@ -18114,7 +18138,7 @@
     </row>
     <row r="767" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="B767" t="s">
         <v>1802</v>
@@ -18128,13 +18152,13 @@
     </row>
     <row r="768" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A768" t="s">
+        <v>2158</v>
+      </c>
+      <c r="B768" t="s">
         <v>2159</v>
       </c>
-      <c r="B768" t="s">
-        <v>2160</v>
-      </c>
       <c r="C768" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="D768" t="s">
         <v>4</v>
@@ -18142,13 +18166,13 @@
     </row>
     <row r="769" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
+        <v>2160</v>
+      </c>
+      <c r="B769" t="s">
         <v>2161</v>
       </c>
-      <c r="B769" t="s">
+      <c r="C769" t="s">
         <v>2162</v>
-      </c>
-      <c r="C769" t="s">
-        <v>2163</v>
       </c>
       <c r="D769" t="s">
         <v>4</v>
@@ -18156,7 +18180,7 @@
     </row>
     <row r="770" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="B770" t="s">
         <v>229</v>
@@ -18170,13 +18194,13 @@
     </row>
     <row r="771" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
+        <v>2164</v>
+      </c>
+      <c r="B771" t="s">
         <v>2165</v>
       </c>
-      <c r="B771" t="s">
+      <c r="C771" t="s">
         <v>2166</v>
-      </c>
-      <c r="C771" t="s">
-        <v>2167</v>
       </c>
       <c r="D771" t="s">
         <v>4</v>
@@ -18184,13 +18208,13 @@
     </row>
     <row r="772" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
+        <v>2167</v>
+      </c>
+      <c r="B772" t="s">
         <v>2168</v>
       </c>
-      <c r="B772" t="s">
+      <c r="C772" t="s">
         <v>2169</v>
-      </c>
-      <c r="C772" t="s">
-        <v>2170</v>
       </c>
       <c r="D772" t="s">
         <v>4</v>
@@ -18198,13 +18222,13 @@
     </row>
     <row r="773" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B773" t="s">
         <v>2171</v>
       </c>
-      <c r="B773" t="s">
+      <c r="C773" t="s">
         <v>2172</v>
-      </c>
-      <c r="C773" t="s">
-        <v>2173</v>
       </c>
       <c r="D773" t="s">
         <v>4</v>
@@ -18212,13 +18236,13 @@
     </row>
     <row r="774" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
+        <v>2173</v>
+      </c>
+      <c r="B774" t="s">
         <v>2174</v>
       </c>
-      <c r="B774" t="s">
+      <c r="C774" t="s">
         <v>2175</v>
-      </c>
-      <c r="C774" t="s">
-        <v>2176</v>
       </c>
       <c r="D774" t="s">
         <v>4</v>
@@ -18226,13 +18250,13 @@
     </row>
     <row r="775" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
+        <v>2176</v>
+      </c>
+      <c r="B775" t="s">
         <v>2177</v>
       </c>
-      <c r="B775" t="s">
+      <c r="C775" t="s">
         <v>2178</v>
-      </c>
-      <c r="C775" t="s">
-        <v>2179</v>
       </c>
       <c r="D775" t="s">
         <v>4</v>
@@ -18240,13 +18264,13 @@
     </row>
     <row r="776" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
+        <v>2179</v>
+      </c>
+      <c r="B776" t="s">
         <v>2180</v>
       </c>
-      <c r="B776" t="s">
+      <c r="C776" t="s">
         <v>2181</v>
-      </c>
-      <c r="C776" t="s">
-        <v>2182</v>
       </c>
       <c r="D776" t="s">
         <v>4</v>
@@ -18254,13 +18278,13 @@
     </row>
     <row r="777" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
+        <v>2182</v>
+      </c>
+      <c r="B777" t="s">
         <v>2183</v>
       </c>
-      <c r="B777" t="s">
+      <c r="C777" t="s">
         <v>2184</v>
-      </c>
-      <c r="C777" t="s">
-        <v>2185</v>
       </c>
       <c r="D777" t="s">
         <v>4</v>
@@ -18268,13 +18292,13 @@
     </row>
     <row r="778" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
+        <v>2185</v>
+      </c>
+      <c r="B778" t="s">
         <v>2186</v>
       </c>
-      <c r="B778" t="s">
+      <c r="C778" t="s">
         <v>2187</v>
-      </c>
-      <c r="C778" t="s">
-        <v>2188</v>
       </c>
       <c r="D778" t="s">
         <v>4</v>
@@ -18282,13 +18306,13 @@
     </row>
     <row r="779" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
+        <v>2188</v>
+      </c>
+      <c r="B779" t="s">
         <v>2189</v>
       </c>
-      <c r="B779" t="s">
+      <c r="C779" t="s">
         <v>2190</v>
-      </c>
-      <c r="C779" t="s">
-        <v>2191</v>
       </c>
       <c r="D779" t="s">
         <v>4</v>
@@ -18296,13 +18320,13 @@
     </row>
     <row r="780" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
+        <v>2191</v>
+      </c>
+      <c r="B780" t="s">
         <v>2192</v>
       </c>
-      <c r="B780" t="s">
+      <c r="C780" t="s">
         <v>2193</v>
-      </c>
-      <c r="C780" t="s">
-        <v>2194</v>
       </c>
       <c r="D780" t="s">
         <v>4</v>
@@ -18310,13 +18334,13 @@
     </row>
     <row r="781" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
+        <v>2194</v>
+      </c>
+      <c r="B781" t="s">
         <v>2195</v>
       </c>
-      <c r="B781" t="s">
+      <c r="C781" t="s">
         <v>2196</v>
-      </c>
-      <c r="C781" t="s">
-        <v>2197</v>
       </c>
       <c r="D781" t="s">
         <v>4</v>
@@ -18324,13 +18348,13 @@
     </row>
     <row r="782" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
+        <v>2197</v>
+      </c>
+      <c r="B782" t="s">
         <v>2198</v>
       </c>
-      <c r="B782" t="s">
+      <c r="C782" t="s">
         <v>2199</v>
-      </c>
-      <c r="C782" t="s">
-        <v>2200</v>
       </c>
       <c r="D782" t="s">
         <v>4</v>
@@ -18338,13 +18362,13 @@
     </row>
     <row r="783" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
+        <v>2200</v>
+      </c>
+      <c r="B783" t="s">
         <v>2201</v>
       </c>
-      <c r="B783" t="s">
+      <c r="C783" t="s">
         <v>2202</v>
-      </c>
-      <c r="C783" t="s">
-        <v>2203</v>
       </c>
       <c r="D783" t="s">
         <v>4</v>
@@ -18352,13 +18376,13 @@
     </row>
     <row r="784" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
+        <v>2203</v>
+      </c>
+      <c r="B784" t="s">
         <v>2204</v>
       </c>
-      <c r="B784" t="s">
+      <c r="C784" t="s">
         <v>2205</v>
-      </c>
-      <c r="C784" t="s">
-        <v>2206</v>
       </c>
       <c r="D784" t="s">
         <v>4</v>
@@ -18366,13 +18390,13 @@
     </row>
     <row r="785" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
+        <v>2206</v>
+      </c>
+      <c r="B785" t="s">
         <v>2207</v>
       </c>
-      <c r="B785" t="s">
+      <c r="C785" t="s">
         <v>2208</v>
-      </c>
-      <c r="C785" t="s">
-        <v>2209</v>
       </c>
       <c r="D785" t="s">
         <v>4</v>
@@ -18380,13 +18404,13 @@
     </row>
     <row r="786" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
+        <v>2209</v>
+      </c>
+      <c r="B786" t="s">
         <v>2210</v>
       </c>
-      <c r="B786" t="s">
+      <c r="C786" t="s">
         <v>2211</v>
-      </c>
-      <c r="C786" t="s">
-        <v>2212</v>
       </c>
       <c r="D786" t="s">
         <v>4</v>
@@ -18394,13 +18418,13 @@
     </row>
     <row r="787" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
+        <v>2212</v>
+      </c>
+      <c r="B787" t="s">
         <v>2213</v>
       </c>
-      <c r="B787" t="s">
+      <c r="C787" t="s">
         <v>2214</v>
-      </c>
-      <c r="C787" t="s">
-        <v>2215</v>
       </c>
       <c r="D787" t="s">
         <v>4</v>
@@ -18408,13 +18432,13 @@
     </row>
     <row r="788" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
+        <v>2215</v>
+      </c>
+      <c r="B788" t="s">
         <v>2216</v>
       </c>
-      <c r="B788" t="s">
+      <c r="C788" t="s">
         <v>2217</v>
-      </c>
-      <c r="C788" t="s">
-        <v>2218</v>
       </c>
       <c r="D788" t="s">
         <v>4</v>
@@ -18422,13 +18446,13 @@
     </row>
     <row r="789" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B789" t="s">
         <v>2219</v>
       </c>
-      <c r="B789" t="s">
+      <c r="C789" t="s">
         <v>2220</v>
-      </c>
-      <c r="C789" t="s">
-        <v>2221</v>
       </c>
       <c r="D789" t="s">
         <v>4</v>
@@ -18436,13 +18460,13 @@
     </row>
     <row r="790" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
+        <v>2221</v>
+      </c>
+      <c r="B790" t="s">
         <v>2222</v>
       </c>
-      <c r="B790" t="s">
+      <c r="C790" t="s">
         <v>2223</v>
-      </c>
-      <c r="C790" t="s">
-        <v>2224</v>
       </c>
       <c r="D790" t="s">
         <v>4</v>
@@ -18450,13 +18474,13 @@
     </row>
     <row r="791" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
+        <v>2224</v>
+      </c>
+      <c r="B791" t="s">
         <v>2225</v>
       </c>
-      <c r="B791" t="s">
+      <c r="C791" t="s">
         <v>2226</v>
-      </c>
-      <c r="C791" t="s">
-        <v>2227</v>
       </c>
       <c r="D791" t="s">
         <v>4</v>
@@ -18464,13 +18488,13 @@
     </row>
     <row r="792" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
+        <v>2227</v>
+      </c>
+      <c r="B792" t="s">
         <v>2228</v>
       </c>
-      <c r="B792" t="s">
+      <c r="C792" t="s">
         <v>2229</v>
-      </c>
-      <c r="C792" t="s">
-        <v>2230</v>
       </c>
       <c r="D792" t="s">
         <v>4</v>
@@ -18478,13 +18502,13 @@
     </row>
     <row r="793" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
+        <v>2230</v>
+      </c>
+      <c r="B793" t="s">
         <v>2231</v>
       </c>
-      <c r="B793" t="s">
+      <c r="C793" t="s">
         <v>2232</v>
-      </c>
-      <c r="C793" t="s">
-        <v>2233</v>
       </c>
       <c r="D793" t="s">
         <v>4</v>
@@ -18492,13 +18516,13 @@
     </row>
     <row r="794" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
+        <v>2233</v>
+      </c>
+      <c r="B794" t="s">
         <v>2234</v>
       </c>
-      <c r="B794" t="s">
+      <c r="C794" t="s">
         <v>2235</v>
-      </c>
-      <c r="C794" t="s">
-        <v>2236</v>
       </c>
       <c r="D794" t="s">
         <v>4</v>
@@ -18506,13 +18530,13 @@
     </row>
     <row r="795" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
+        <v>2236</v>
+      </c>
+      <c r="B795" t="s">
         <v>2237</v>
       </c>
-      <c r="B795" t="s">
+      <c r="C795" t="s">
         <v>2238</v>
-      </c>
-      <c r="C795" t="s">
-        <v>2239</v>
       </c>
       <c r="D795" t="s">
         <v>4</v>
@@ -18520,13 +18544,13 @@
     </row>
     <row r="796" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
+        <v>2239</v>
+      </c>
+      <c r="B796" t="s">
         <v>2240</v>
       </c>
-      <c r="B796" t="s">
+      <c r="C796" t="s">
         <v>2241</v>
-      </c>
-      <c r="C796" t="s">
-        <v>2242</v>
       </c>
       <c r="D796" t="s">
         <v>4</v>
@@ -18534,13 +18558,13 @@
     </row>
     <row r="797" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B797" t="s">
         <v>2243</v>
       </c>
-      <c r="B797" t="s">
+      <c r="C797" t="s">
         <v>2244</v>
-      </c>
-      <c r="C797" t="s">
-        <v>2245</v>
       </c>
       <c r="D797" t="s">
         <v>4</v>
@@ -18548,13 +18572,13 @@
     </row>
     <row r="798" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
+        <v>2245</v>
+      </c>
+      <c r="B798" t="s">
         <v>2246</v>
       </c>
-      <c r="B798" t="s">
+      <c r="C798" t="s">
         <v>2247</v>
-      </c>
-      <c r="C798" t="s">
-        <v>2248</v>
       </c>
       <c r="D798" t="s">
         <v>4</v>
@@ -18562,13 +18586,13 @@
     </row>
     <row r="799" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B799" t="s">
         <v>2249</v>
       </c>
-      <c r="B799" t="s">
+      <c r="C799" t="s">
         <v>2250</v>
-      </c>
-      <c r="C799" t="s">
-        <v>2251</v>
       </c>
       <c r="D799" t="s">
         <v>4</v>
@@ -18576,13 +18600,13 @@
     </row>
     <row r="800" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B800" t="s">
         <v>2252</v>
       </c>
-      <c r="B800" t="s">
+      <c r="C800" t="s">
         <v>2253</v>
-      </c>
-      <c r="C800" t="s">
-        <v>2254</v>
       </c>
       <c r="D800" t="s">
         <v>4</v>
@@ -18590,13 +18614,13 @@
     </row>
     <row r="801" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
+        <v>2254</v>
+      </c>
+      <c r="B801" t="s">
         <v>2255</v>
       </c>
-      <c r="B801" t="s">
-        <v>2256</v>
-      </c>
       <c r="C801" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="D801" t="s">
         <v>4</v>
@@ -18604,13 +18628,13 @@
     </row>
     <row r="802" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
+        <v>2256</v>
+      </c>
+      <c r="B802" t="s">
         <v>2257</v>
       </c>
-      <c r="B802" t="s">
+      <c r="C802" t="s">
         <v>2258</v>
-      </c>
-      <c r="C802" t="s">
-        <v>2259</v>
       </c>
       <c r="D802" t="s">
         <v>4</v>
@@ -18618,13 +18642,13 @@
     </row>
     <row r="803" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
+        <v>2259</v>
+      </c>
+      <c r="B803" t="s">
         <v>2260</v>
       </c>
-      <c r="B803" t="s">
+      <c r="C803" t="s">
         <v>2261</v>
-      </c>
-      <c r="C803" t="s">
-        <v>2262</v>
       </c>
       <c r="D803" t="s">
         <v>4</v>
@@ -18632,13 +18656,13 @@
     </row>
     <row r="804" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
+        <v>2262</v>
+      </c>
+      <c r="B804" t="s">
         <v>2263</v>
       </c>
-      <c r="B804" t="s">
+      <c r="C804" t="s">
         <v>2264</v>
-      </c>
-      <c r="C804" t="s">
-        <v>2265</v>
       </c>
       <c r="D804" t="s">
         <v>4</v>
@@ -18646,13 +18670,13 @@
     </row>
     <row r="805" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B805" t="s">
         <v>2266</v>
       </c>
-      <c r="B805" t="s">
+      <c r="C805" t="s">
         <v>2267</v>
-      </c>
-      <c r="C805" t="s">
-        <v>2268</v>
       </c>
       <c r="D805" t="s">
         <v>4</v>
@@ -18660,13 +18684,13 @@
     </row>
     <row r="806" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B806" t="s">
         <v>2269</v>
       </c>
-      <c r="B806" t="s">
+      <c r="C806" t="s">
         <v>2270</v>
-      </c>
-      <c r="C806" t="s">
-        <v>2271</v>
       </c>
       <c r="D806" t="s">
         <v>4</v>
@@ -18674,13 +18698,13 @@
     </row>
     <row r="807" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
+        <v>2271</v>
+      </c>
+      <c r="B807" t="s">
         <v>2272</v>
       </c>
-      <c r="B807" t="s">
+      <c r="C807" t="s">
         <v>2273</v>
-      </c>
-      <c r="C807" t="s">
-        <v>2274</v>
       </c>
       <c r="D807" t="s">
         <v>4</v>
@@ -18688,13 +18712,13 @@
     </row>
     <row r="808" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
+        <v>2274</v>
+      </c>
+      <c r="B808" t="s">
         <v>2275</v>
       </c>
-      <c r="B808" t="s">
+      <c r="C808" t="s">
         <v>2276</v>
-      </c>
-      <c r="C808" t="s">
-        <v>2277</v>
       </c>
       <c r="D808" t="s">
         <v>4</v>
@@ -18702,13 +18726,13 @@
     </row>
     <row r="809" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
-        <v>2278</v>
+        <v>2277</v>
       </c>
       <c r="B809" t="s">
+        <v>2252</v>
+      </c>
+      <c r="C809" t="s">
         <v>2253</v>
-      </c>
-      <c r="C809" t="s">
-        <v>2254</v>
       </c>
       <c r="D809" t="s">
         <v>4</v>
@@ -18716,13 +18740,13 @@
     </row>
     <row r="810" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A810" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B810" t="s">
         <v>2279</v>
       </c>
-      <c r="B810" t="s">
+      <c r="C810" t="s">
         <v>2280</v>
-      </c>
-      <c r="C810" t="s">
-        <v>2281</v>
       </c>
       <c r="D810" t="s">
         <v>4</v>
@@ -18730,13 +18754,13 @@
     </row>
     <row r="811" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
+        <v>2281</v>
+      </c>
+      <c r="B811" t="s">
         <v>2282</v>
       </c>
-      <c r="B811" t="s">
+      <c r="C811" t="s">
         <v>2283</v>
-      </c>
-      <c r="C811" t="s">
-        <v>2284</v>
       </c>
       <c r="D811" t="s">
         <v>4</v>
@@ -18744,13 +18768,13 @@
     </row>
     <row r="812" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B812" t="s">
         <v>2285</v>
       </c>
-      <c r="B812" t="s">
+      <c r="C812" t="s">
         <v>2286</v>
-      </c>
-      <c r="C812" t="s">
-        <v>2287</v>
       </c>
       <c r="D812" t="s">
         <v>4</v>
@@ -18758,13 +18782,13 @@
     </row>
     <row r="813" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
+        <v>2287</v>
+      </c>
+      <c r="B813" t="s">
         <v>2288</v>
       </c>
-      <c r="B813" t="s">
+      <c r="C813" t="s">
         <v>2289</v>
-      </c>
-      <c r="C813" t="s">
-        <v>2290</v>
       </c>
       <c r="D813" t="s">
         <v>4</v>
@@ -18772,13 +18796,13 @@
     </row>
     <row r="814" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A814" t="s">
+        <v>2290</v>
+      </c>
+      <c r="B814" t="s">
         <v>2291</v>
       </c>
-      <c r="B814" t="s">
+      <c r="C814" t="s">
         <v>2292</v>
-      </c>
-      <c r="C814" t="s">
-        <v>2293</v>
       </c>
       <c r="D814" t="s">
         <v>4</v>
@@ -18786,7 +18810,7 @@
     </row>
     <row r="815" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A815" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="B815" t="s">
         <v>2091</v>
@@ -18800,13 +18824,13 @@
     </row>
     <row r="816" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A816" t="s">
+        <v>2294</v>
+      </c>
+      <c r="B816" t="s">
         <v>2295</v>
       </c>
-      <c r="B816" t="s">
+      <c r="C816" t="s">
         <v>2296</v>
-      </c>
-      <c r="C816" t="s">
-        <v>2297</v>
       </c>
       <c r="D816" t="s">
         <v>4</v>
@@ -18814,13 +18838,13 @@
     </row>
     <row r="817" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
+        <v>2297</v>
+      </c>
+      <c r="B817" t="s">
         <v>2298</v>
       </c>
-      <c r="B817" t="s">
+      <c r="C817" t="s">
         <v>2299</v>
-      </c>
-      <c r="C817" t="s">
-        <v>2300</v>
       </c>
       <c r="D817" t="s">
         <v>4</v>
@@ -18828,13 +18852,13 @@
     </row>
     <row r="818" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A818" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B818" t="s">
         <v>2301</v>
       </c>
-      <c r="B818" t="s">
+      <c r="C818" t="s">
         <v>2302</v>
-      </c>
-      <c r="C818" t="s">
-        <v>2303</v>
       </c>
       <c r="D818" t="s">
         <v>4</v>
@@ -18842,13 +18866,13 @@
     </row>
     <row r="819" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A819" t="s">
+        <v>2303</v>
+      </c>
+      <c r="B819" t="s">
         <v>2304</v>
       </c>
-      <c r="B819" t="s">
+      <c r="C819" t="s">
         <v>2305</v>
-      </c>
-      <c r="C819" t="s">
-        <v>2306</v>
       </c>
       <c r="D819" t="s">
         <v>4</v>
@@ -18856,13 +18880,13 @@
     </row>
     <row r="820" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A820" t="s">
+        <v>2306</v>
+      </c>
+      <c r="B820" t="s">
         <v>2307</v>
       </c>
-      <c r="B820" t="s">
+      <c r="C820" t="s">
         <v>2308</v>
-      </c>
-      <c r="C820" t="s">
-        <v>2309</v>
       </c>
       <c r="D820" t="s">
         <v>4</v>
@@ -18870,13 +18894,13 @@
     </row>
     <row r="821" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A821" t="s">
+        <v>2309</v>
+      </c>
+      <c r="B821" t="s">
         <v>2310</v>
       </c>
-      <c r="B821" t="s">
+      <c r="C821" t="s">
         <v>2311</v>
-      </c>
-      <c r="C821" t="s">
-        <v>2312</v>
       </c>
       <c r="D821" t="s">
         <v>4</v>
@@ -18884,13 +18908,13 @@
     </row>
     <row r="822" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A822" t="s">
+        <v>2312</v>
+      </c>
+      <c r="B822" t="s">
         <v>2313</v>
       </c>
-      <c r="B822" t="s">
+      <c r="C822" t="s">
         <v>2314</v>
-      </c>
-      <c r="C822" t="s">
-        <v>2315</v>
       </c>
       <c r="D822" t="s">
         <v>4</v>
@@ -18898,13 +18922,13 @@
     </row>
     <row r="823" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A823" t="s">
+        <v>2315</v>
+      </c>
+      <c r="B823" t="s">
         <v>2316</v>
       </c>
-      <c r="B823" t="s">
+      <c r="C823" t="s">
         <v>2317</v>
-      </c>
-      <c r="C823" t="s">
-        <v>2318</v>
       </c>
       <c r="D823" t="s">
         <v>4</v>
@@ -18912,13 +18936,13 @@
     </row>
     <row r="824" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A824" t="s">
+        <v>2318</v>
+      </c>
+      <c r="B824" t="s">
         <v>2319</v>
       </c>
-      <c r="B824" t="s">
+      <c r="C824" t="s">
         <v>2320</v>
-      </c>
-      <c r="C824" t="s">
-        <v>2321</v>
       </c>
       <c r="D824" t="s">
         <v>4</v>
@@ -18926,13 +18950,13 @@
     </row>
     <row r="825" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A825" t="s">
+        <v>2321</v>
+      </c>
+      <c r="B825" t="s">
         <v>2322</v>
       </c>
-      <c r="B825" t="s">
+      <c r="C825" t="s">
         <v>2323</v>
-      </c>
-      <c r="C825" t="s">
-        <v>2324</v>
       </c>
       <c r="D825" t="s">
         <v>4</v>
@@ -18940,13 +18964,13 @@
     </row>
     <row r="826" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A826" t="s">
+        <v>2324</v>
+      </c>
+      <c r="B826" t="s">
         <v>2325</v>
       </c>
-      <c r="B826" t="s">
+      <c r="C826" t="s">
         <v>2326</v>
-      </c>
-      <c r="C826" t="s">
-        <v>2327</v>
       </c>
       <c r="D826" t="s">
         <v>4</v>
@@ -18954,13 +18978,13 @@
     </row>
     <row r="827" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A827" t="s">
+        <v>2327</v>
+      </c>
+      <c r="B827" t="s">
         <v>2328</v>
       </c>
-      <c r="B827" t="s">
+      <c r="C827" t="s">
         <v>2329</v>
-      </c>
-      <c r="C827" t="s">
-        <v>2330</v>
       </c>
       <c r="D827" t="s">
         <v>4</v>
@@ -18968,13 +18992,13 @@
     </row>
     <row r="828" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A828" t="s">
+        <v>2330</v>
+      </c>
+      <c r="B828" t="s">
         <v>2331</v>
       </c>
-      <c r="B828" t="s">
+      <c r="C828" t="s">
         <v>2332</v>
-      </c>
-      <c r="C828" t="s">
-        <v>2333</v>
       </c>
       <c r="D828" t="s">
         <v>4</v>
@@ -18982,13 +19006,13 @@
     </row>
     <row r="829" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A829" t="s">
+        <v>2333</v>
+      </c>
+      <c r="B829" t="s">
         <v>2334</v>
       </c>
-      <c r="B829" t="s">
+      <c r="C829" t="s">
         <v>2335</v>
-      </c>
-      <c r="C829" t="s">
-        <v>2336</v>
       </c>
       <c r="D829" t="s">
         <v>4</v>
@@ -18996,13 +19020,13 @@
     </row>
     <row r="830" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A830" t="s">
+        <v>2336</v>
+      </c>
+      <c r="B830" t="s">
         <v>2337</v>
       </c>
-      <c r="B830" t="s">
+      <c r="C830" t="s">
         <v>2338</v>
-      </c>
-      <c r="C830" t="s">
-        <v>2339</v>
       </c>
       <c r="D830" t="s">
         <v>4</v>
@@ -19010,7 +19034,7 @@
     </row>
     <row r="831" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="B831" t="s">
         <v>2094</v>
@@ -19024,35 +19048,35 @@
     </row>
     <row r="832" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
+        <v>2340</v>
+      </c>
+      <c r="B832" t="s">
         <v>2341</v>
       </c>
-      <c r="B832" t="s">
+      <c r="C832" t="s">
         <v>2342</v>
       </c>
-      <c r="C832" t="s">
+      <c r="D832" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="833" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A833" t="s">
         <v>2343</v>
       </c>
-      <c r="D832" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="833" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A833" t="s">
+      <c r="B833" t="s">
         <v>2344</v>
       </c>
-      <c r="B833" t="s">
+      <c r="C833" t="s">
         <v>2345</v>
       </c>
-      <c r="C833" t="s">
+      <c r="D833" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="834" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A834" t="s">
         <v>2346</v>
-      </c>
-      <c r="D833" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="834" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A834" t="s">
-        <v>2347</v>
       </c>
       <c r="B834" t="s">
         <v>1750</v>
@@ -19064,37 +19088,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="835" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
+        <v>2347</v>
+      </c>
+      <c r="B835" t="s">
         <v>2348</v>
       </c>
-      <c r="B835" t="s">
+      <c r="C835" t="s">
         <v>2349</v>
       </c>
-      <c r="C835" t="s">
+      <c r="D835" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="836" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A836" t="s">
         <v>2350</v>
       </c>
-      <c r="D835" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="836" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A836" t="s">
+      <c r="B836" t="s">
         <v>2351</v>
       </c>
-      <c r="B836" t="s">
+      <c r="C836" t="s">
         <v>2352</v>
       </c>
-      <c r="C836" t="s">
+      <c r="D836" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="837" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A837" t="s">
         <v>2353</v>
-      </c>
-      <c r="D836" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="837" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A837" t="s">
-        <v>2354</v>
       </c>
       <c r="B837" t="s">
         <v>1762</v>
@@ -19106,23 +19130,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="838" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
+        <v>2354</v>
+      </c>
+      <c r="B838" t="s">
         <v>2355</v>
       </c>
-      <c r="B838" t="s">
+      <c r="C838" t="s">
         <v>2356</v>
       </c>
-      <c r="C838" t="s">
+      <c r="D838" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="839" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A839" t="s">
         <v>2357</v>
-      </c>
-      <c r="D838" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="839" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A839" t="s">
-        <v>2358</v>
       </c>
       <c r="B839" t="s">
         <v>1767</v>
@@ -19132,6 +19156,78 @@
       </c>
       <c r="D839" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="841" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A841" t="s">
+        <v>2358</v>
+      </c>
+      <c r="B841" t="s">
+        <v>33</v>
+      </c>
+      <c r="C841" t="s">
+        <v>33</v>
+      </c>
+      <c r="D841" t="s">
+        <v>4</v>
+      </c>
+      <c r="E841" t="str">
+        <f>"{{dictionary."&amp;A841&amp;"}}"</f>
+        <v>{{dictionary.vixiCsCompliance}}</v>
+      </c>
+    </row>
+    <row r="842" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A842" t="s">
+        <v>2362</v>
+      </c>
+      <c r="B842" t="s">
+        <v>34</v>
+      </c>
+      <c r="C842" t="s">
+        <v>88</v>
+      </c>
+      <c r="D842" t="s">
+        <v>4</v>
+      </c>
+      <c r="E842" t="str">
+        <f t="shared" ref="E842:E844" si="0">"{{dictionary."&amp;A842&amp;"}}"</f>
+        <v>{{dictionary.vixiCsSeguranca}}</v>
+      </c>
+    </row>
+    <row r="843" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A843" t="s">
+        <v>2363</v>
+      </c>
+      <c r="B843" t="s">
+        <v>2360</v>
+      </c>
+      <c r="C843" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D843" t="s">
+        <v>4</v>
+      </c>
+      <c r="E843" t="str">
+        <f t="shared" si="0"/>
+        <v>{{dictionary.vixiCsPoliticas}}</v>
+      </c>
+    </row>
+    <row r="844" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A844" t="s">
+        <v>2359</v>
+      </c>
+      <c r="B844" t="s">
+        <v>2364</v>
+      </c>
+      <c r="C844" t="s">
+        <v>2365</v>
+      </c>
+      <c r="D844" t="s">
+        <v>4</v>
+      </c>
+      <c r="E844" t="str">
+        <f t="shared" si="0"/>
+        <v>{{dictionary.vixiCsProcedimentos}}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arquivo de tradução atualizado
</commit_message>
<xml_diff>
--- a/database/translations.xlsx
+++ b/database/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\leebank\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\leebank\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B797210B-4B46-43AB-9445-3E59D309DBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FE78D8-605A-4B0D-A884-75557456EE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{76BFD47B-F395-40CE-A23A-1FAE0D23D331}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{76BFD47B-F395-40CE-A23A-1FAE0D23D331}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -7496,10 +7496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02064365-2FF8-4B03-A006-514EE9525724}">
-  <dimension ref="A1:E844"/>
+  <dimension ref="A1:D844"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A742" workbookViewId="0">
-      <selection activeCell="A750" sqref="A750"/>
+    <sheetView tabSelected="1" topLeftCell="A835" workbookViewId="0">
+      <selection activeCell="E841" sqref="E841:E844"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19060,7 +19060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="833" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="833" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
         <v>2343</v>
       </c>
@@ -19074,7 +19074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="834" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="834" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
         <v>2346</v>
       </c>
@@ -19088,7 +19088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="835" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
         <v>2347</v>
       </c>
@@ -19102,7 +19102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="836" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="836" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
         <v>2350</v>
       </c>
@@ -19116,7 +19116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="837" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="837" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
         <v>2353</v>
       </c>
@@ -19130,7 +19130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="838" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
         <v>2354</v>
       </c>
@@ -19144,7 +19144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="839" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
         <v>2357</v>
       </c>
@@ -19158,7 +19158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="841" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
         <v>2358</v>
       </c>
@@ -19171,12 +19171,8 @@
       <c r="D841" t="s">
         <v>4</v>
       </c>
-      <c r="E841" t="str">
-        <f>"{{dictionary."&amp;A841&amp;"}}"</f>
-        <v>{{dictionary.vixiCsCompliance}}</v>
-      </c>
-    </row>
-    <row r="842" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="842" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
         <v>2362</v>
       </c>
@@ -19189,12 +19185,8 @@
       <c r="D842" t="s">
         <v>4</v>
       </c>
-      <c r="E842" t="str">
-        <f t="shared" ref="E842:E844" si="0">"{{dictionary."&amp;A842&amp;"}}"</f>
-        <v>{{dictionary.vixiCsSeguranca}}</v>
-      </c>
-    </row>
-    <row r="843" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="843" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
         <v>2363</v>
       </c>
@@ -19207,12 +19199,8 @@
       <c r="D843" t="s">
         <v>4</v>
       </c>
-      <c r="E843" t="str">
-        <f t="shared" si="0"/>
-        <v>{{dictionary.vixiCsPoliticas}}</v>
-      </c>
-    </row>
-    <row r="844" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="844" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
         <v>2359</v>
       </c>
@@ -19224,10 +19212,6 @@
       </c>
       <c r="D844" t="s">
         <v>4</v>
-      </c>
-      <c r="E844" t="str">
-        <f t="shared" si="0"/>
-        <v>{{dictionary.vixiCsProcedimentos}}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>